<commit_message>
test: add unit tests for project
</commit_message>
<xml_diff>
--- a/data/Tasks.xlsx
+++ b/data/Tasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\rss-mentor-dashboard-bootstrap-master\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\git\rss-mentor-dashboard-server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -78,9 +78,6 @@
     <t>надо будет скоро сделать</t>
   </si>
   <si>
-    <t xml:space="preserve">RS Activist - </t>
-  </si>
-  <si>
     <t>https://github.com/rolling-scopes-school/tasks/blob/2018-Q3/tasks/rs-school-activist.md</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>https://github.com/rolling-scopes-school/tasks/blob/2018-Q3/tasks/youtube.md</t>
   </si>
   <si>
-    <t>CodeJam "Scoreboard"</t>
-  </si>
-  <si>
     <t>https://github.com/rolling-scopes-school/tasks/blob/2018-Q3/tasks/codejam-scoreboard.md</t>
   </si>
   <si>
@@ -103,6 +97,12 @@
   </si>
   <si>
     <t>Course work</t>
+  </si>
+  <si>
+    <t>RS Activist</t>
+  </si>
+  <si>
+    <t>Code Jam "Scoreboard"</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -539,10 +539,10 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -550,10 +550,10 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -572,10 +572,10 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>

</xml_diff>